<commit_message>
add Abbyy embedded OCR
</commit_message>
<xml_diff>
--- a/Output/Invoice_Verztec_output.xlsx
+++ b/Output/Invoice_Verztec_output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <x:si>
     <x:t>name</x:t>
   </x:si>
@@ -31,51 +31,21 @@
     <x:t>billing-addr</x:t>
   </x:si>
   <x:si>
-    <x:t>shipping-addr</x:t>
-  </x:si>
-  <x:si>
     <x:t>invoice-no</x:t>
   </x:si>
   <x:si>
-    <x:t>po-no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>vendor-vat-no</x:t>
-  </x:si>
-  <x:si>
     <x:t>date</x:t>
   </x:si>
   <x:si>
-    <x:t>tax</x:t>
-  </x:si>
-  <x:si>
     <x:t>total</x:t>
   </x:si>
   <x:si>
-    <x:t>payment-terms</x:t>
-  </x:si>
-  <x:si>
     <x:t>net-amount</x:t>
   </x:si>
   <x:si>
-    <x:t>due-date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>discount</x:t>
-  </x:si>
-  <x:si>
-    <x:t>shipping-charges</x:t>
-  </x:si>
-  <x:si>
-    <x:t>payment-addr</x:t>
-  </x:si>
-  <x:si>
     <x:t>items</x:t>
   </x:si>
   <x:si>
-    <x:t>currency</x:t>
-  </x:si>
-  <x:si>
     <x:t>Verztec Consulting (Thailand) Ltd,</x:t>
   </x:si>
   <x:si>
@@ -94,9 +64,6 @@
     <x:t>2020-06-29</x:t>
   </x:si>
   <x:si>
-    <x:t>2943.925</x:t>
-  </x:si>
-  <x:si>
     <x:t>45000.000</x:t>
   </x:si>
   <x:si>
@@ -106,34 +73,13 @@
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>INR</x:t>
-  </x:si>
-  <x:si>
     <x:t>description</x:t>
   </x:si>
   <x:si>
-    <x:t>quantity</x:t>
-  </x:si>
-  <x:si>
-    <x:t>unit-price</x:t>
-  </x:si>
-  <x:si>
     <x:t>line-amount</x:t>
   </x:si>
   <x:si>
-    <x:t>item-po-no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>line-no</x:t>
-  </x:si>
-  <x:si>
-    <x:t>part-no</x:t>
-  </x:si>
-  <x:si>
     <x:t>50% Deposit Fee Produciton Course of Digital Learning .5 steps of IBE Competency Included</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -484,13 +430,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:S2"/>
+  <x:dimension ref="A1:I2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:19">
+    <x:row r="1" spans="1:9">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -518,70 +464,34 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:9">
+      <x:c r="A2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M1" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N1" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="O1" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P1" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="Q1" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="R1" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="S1" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:19">
-      <x:c r="A2" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="K2" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="R2" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="S2" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -598,13 +508,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:S2"/>
+  <x:dimension ref="A1:I2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:19">
+    <x:row r="1" spans="1:9">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -632,70 +542,34 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:9">
+      <x:c r="A2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M1" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N1" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="O1" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P1" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="Q1" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="R1" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="S1" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:19">
-      <x:c r="A2" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="K2" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="R2" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="S2" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -712,47 +586,26 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G2"/>
+  <x:dimension ref="A1:B2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:2">
       <x:c r="A1" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
       <x:c r="A2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -769,47 +622,26 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G2"/>
+  <x:dimension ref="A1:B2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:2">
       <x:c r="A1" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
       <x:c r="A2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
use Google OCR instead
</commit_message>
<xml_diff>
--- a/Output/Invoice_Verztec_output.xlsx
+++ b/Output/Invoice_Verztec_output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <x:si>
     <x:t>name</x:t>
   </x:si>
@@ -28,6 +28,9 @@
     <x:t>billing-name</x:t>
   </x:si>
   <x:si>
+    <x:t>tax-id</x:t>
+  </x:si>
+  <x:si>
     <x:t>billing-addr</x:t>
   </x:si>
   <x:si>
@@ -52,10 +55,13 @@
     <x:t>1 Empire Tower, 45th Floor, Unit 4505 River Wing West, South Sathorn Road Yannawa Sub-district, Sathorn District Bangkok 10120 Thailand</x:t>
   </x:si>
   <x:si>
-    <x:t>Verztec Consulting (Thailand) Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1 Empire Tower, 45th Floor, Unit 4505 River Wing West, South Sathorn Road. Yannawa Sub-district, Sathorn District,</x:t>
+    <x:t>บริษัท เอสซีจี เคมิคอลส์ จำกัด (สำนักงานใหญ่)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0105538052728</x:t>
+  </x:si>
+  <x:si>
+    <x:t>เลขที่ 1 ถ.ปูนซิเมนต์ไทย บางซื่อ กรุงเทพฯ 10800</x:t>
   </x:si>
   <x:si>
     <x:t>RC2020/06/003053</x:t>
@@ -76,10 +82,19 @@
     <x:t>description</x:t>
   </x:si>
   <x:si>
+    <x:t>quantity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>unit-price</x:t>
+  </x:si>
+  <x:si>
     <x:t>line-amount</x:t>
   </x:si>
   <x:si>
-    <x:t>50% Deposit Fee Produciton Course of Digital Learning .5 steps of IBE Competency Included</x:t>
+    <x:t>50% Deposit Fee Produciton Course of Digital Learning 5 steps of IBE Competency Project Managemnet Fee Included</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -436,7 +451,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:10">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -464,34 +479,40 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:9">
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:10">
       <x:c r="A2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>19</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -514,7 +535,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:10">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -542,34 +563,40 @@
       <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:9">
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:10">
       <x:c r="A2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="H2" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>19</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -592,20 +619,29 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
-      <x:c r="A2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -628,20 +664,29 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:4">
       <x:c r="A1" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
-      <x:c r="A2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>